<commit_message>
master planDemoCooking and DeletePhone on pasar
</commit_message>
<xml_diff>
--- a/public/assets/PasarImport.xlsx
+++ b/public/assets/PasarImport.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>AREA</t>
   </si>
@@ -28,9 +28,6 @@
   </si>
   <si>
     <t>PASAR</t>
-  </si>
-  <si>
-    <t>PHONE</t>
   </si>
   <si>
     <t>ADDRESS</t>
@@ -372,7 +369,7 @@
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -397,14 +394,12 @@
         <v>6</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="H1" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>